<commit_message>
coherence update and new MP assignment rules
</commit_message>
<xml_diff>
--- a/4.Xenium/SampleIdentifier.xlsx
+++ b/4.Xenium/SampleIdentifier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sdaniell/Partners HealthCare Dropbox/Sara Danielli/Sara Danielli/Project/Ependymoma/12 - Xenium/scripts_revisions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E08544-788A-5B42-A73B-3FB9BDCFDEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221C0F92-FEAC-3C46-9E1C-81A5F76EB202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5780" yWindow="760" windowWidth="16840" windowHeight="17820" xr2:uid="{A559A398-72E6-E042-8621-8F87017513BB}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
   <si>
     <t>20231020__200939__BT2126_BT1745</t>
   </si>
@@ -276,6 +276,33 @@
   </si>
   <si>
     <t>STEPN15_Region_1</t>
+  </si>
+  <si>
+    <t>Resolution</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.2</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.5</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.7</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.3</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.4</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.8</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.0.9</t>
+  </si>
+  <si>
+    <t>SCT_snn_res.1</t>
   </si>
 </sst>
 </file>
@@ -330,13 +357,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC6E243-611D-B945-8423-86C321F7EA44}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -684,10 +712,11 @@
     <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="52" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="100.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -706,8 +735,11 @@
       <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -726,8 +758,11 @@
       <c r="F2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -746,8 +781,11 @@
       <c r="F3" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -766,8 +804,11 @@
       <c r="F4" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -786,8 +827,11 @@
       <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -806,8 +850,11 @@
       <c r="F6" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -826,8 +873,11 @@
       <c r="F7" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -846,8 +896,11 @@
       <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -866,8 +919,11 @@
       <c r="F9" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -886,8 +942,11 @@
       <c r="F10" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -906,8 +965,11 @@
       <c r="F11" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -926,8 +988,11 @@
       <c r="F12" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -946,8 +1011,11 @@
       <c r="F13" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -966,8 +1034,11 @@
       <c r="F14" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -986,8 +1057,11 @@
       <c r="F15" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1006,8 +1080,11 @@
       <c r="F16" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1026,8 +1103,11 @@
       <c r="F17" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1046,8 +1126,11 @@
       <c r="F18" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G18" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1066,8 +1149,11 @@
       <c r="F19" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G19" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1086,8 +1172,11 @@
       <c r="F20" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G20" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1106,8 +1195,11 @@
       <c r="F21" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G21" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1126,8 +1218,11 @@
       <c r="F22" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G22" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1146,8 +1241,11 @@
       <c r="F23" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G23" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -1165,6 +1263,9 @@
       </c>
       <c r="F24" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>